<commit_message>
Updating for New Manufacturing Ideas
</commit_message>
<xml_diff>
--- a/BOM/Parts List and Cost Analysis.xlsx
+++ b/BOM/Parts List and Cost Analysis.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tommy Rohmann\OneDrive\Projects\Microgravity-Press-Washing-Machine\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dcdf7eb514dfaeec/Projects/Microgravity-Press-Washing-Machine/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BDCCF2F-CD62-4976-945E-343FBA828B14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
@@ -1447,8 +1447,8 @@
   <dimension ref="A1:O446"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="10" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N24" sqref="N24"/>
+      <pane ySplit="2" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3352,7 +3352,7 @@
       </c>
       <c r="M49" s="3" cm="1">
         <f t="array" aca="1" ref="M49" ca="1">IF(OR(CELL("address")=CELL("address",A49),CELL("address")=CELL("address",B49),CELL("address")=CELL("address",C49),CELL("address")=CELL("address",D49),CELL("address")=CELL("address",E49),CELL("address")=CELL("address",F49),CELL("address")=CELL("address",G49),CELL("address")=CELL("address",H49),CELL("address")=CELL("address",I49)),NOW(),M49)</f>
-        <v>45646.883798726849</v>
+        <v>46026.352704398145</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.45">

</xml_diff>